<commit_message>
Semi USB: checklist: Completed schematic section for PCB Design Checklist for the 1_Interface_Charge_RBF board
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\1_Interface_Charge_RBF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A5BC14-4536-4FDE-B997-264165DAEC2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C0D5C-02AD-4F98-AE82-A75ACD07C9C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="170">
   <si>
     <t>1.</t>
   </si>
@@ -515,16 +515,34 @@
     <t>Done initial placement, waiting avaliation</t>
   </si>
   <si>
-    <t>Not necessary? Maybe for charging batteries indicatot but the device of the charge already has indications so...</t>
-  </si>
-  <si>
     <t>No Integrated Circuits in design</t>
   </si>
   <si>
-    <t>Power supply only needed from msp-fet debugger</t>
-  </si>
-  <si>
     <t>No polarity components</t>
+  </si>
+  <si>
+    <t>Not necessary? Maybe for charging batteries indicatot but the device of the charge already has indications</t>
+  </si>
+  <si>
+    <t>Power supply is provided by the msp-fet JTAG_VCC</t>
+  </si>
+  <si>
+    <t>Same used for the engeenering models</t>
+  </si>
+  <si>
+    <t>Power from debugger must be stable enough</t>
+  </si>
+  <si>
+    <t>No errors found when compiling</t>
+  </si>
+  <si>
+    <t>No high speed signals in design</t>
+  </si>
+  <si>
+    <t>Not needed in this particular board</t>
+  </si>
+  <si>
+    <t>Very simple design (1 sheet)</t>
   </si>
 </sst>
 </file>
@@ -1068,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1133,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43959.712889351853</v>
+        <v>43965.840691550926</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1188,13 +1206,13 @@
       <c r="B8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C8" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1210,7 +1228,7 @@
         <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1226,7 +1244,7 @@
         <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1242,7 +1260,7 @@
         <v>133</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1252,12 +1270,14 @@
       <c r="B12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C12" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
@@ -1286,7 +1306,7 @@
         <v>133</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1301,7 +1321,9 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -1315,7 +1337,9 @@
       <c r="E16" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1357,7 +1381,9 @@
       <c r="E19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
@@ -1380,12 +1406,14 @@
       <c r="B21" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C21" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
@@ -1413,7 +1441,9 @@
       <c r="E23" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">

</xml_diff>

<commit_message>
Semi USB: checklist: Updating all itens on layout section of PCB Design Checklist for 1_Interface_Charge_RBF board
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\1_Interface_Charge_RBF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C0D5C-02AD-4F98-AE82-A75ACD07C9C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA31E61C-648E-434C-BE43-4F16EB04F404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="194">
   <si>
     <t>1.</t>
   </si>
@@ -506,9 +506,6 @@
     <t>Variant: Semi USB - Charge and RBF Interstage Interface Board Nº1</t>
   </si>
   <si>
-    <t>Project: Interstage Interface Board for FloripaSat-2 CubeSat</t>
-  </si>
-  <si>
     <t>Since the PCB is a interface for flashing and debugging this is not needed</t>
   </si>
   <si>
@@ -543,6 +540,81 @@
   </si>
   <si>
     <t>Very simple design (1 sheet)</t>
+  </si>
+  <si>
+    <t>Need double check after review</t>
+  </si>
+  <si>
+    <t>Used direct contact on power and GND nets</t>
+  </si>
+  <si>
+    <t>See if the PCB manufacture have an acceptable hole size tolerance for connectors</t>
+  </si>
+  <si>
+    <t>Just a bit off in the 3D models for the pin header but not critical</t>
+  </si>
+  <si>
+    <t>Used polygons</t>
+  </si>
+  <si>
+    <t>Used standard 0.508mm to RBF and 0.254mm to all other ones (same as EPS module)</t>
+  </si>
+  <si>
+    <t>Used at the moment 0.15mm from JLCPCB capabilities</t>
+  </si>
+  <si>
+    <t>Waiting final "martelada"</t>
+  </si>
+  <si>
+    <t>Simple 1,6mm thick double layer board design</t>
+  </si>
+  <si>
+    <t>No analog and digital concerns for this simple board design</t>
+  </si>
+  <si>
+    <t>Used standard 1oz (0.035mm) to copper traces</t>
+  </si>
+  <si>
+    <t>Heavier components needs to be on top layer for AIT reasons</t>
+  </si>
+  <si>
+    <t>Needs some revision</t>
+  </si>
+  <si>
+    <t>Project: Interstage Interface Panel for FloripaSat-2 CubeSat</t>
+  </si>
+  <si>
+    <t>Simple 2 layer pcb design</t>
+  </si>
+  <si>
+    <t>Extra empty column called "Board Layer Stack"</t>
+  </si>
+  <si>
+    <t>Only 1 plane GND on top layer used (2 layer design)</t>
+  </si>
+  <si>
+    <t>Opted for direct contact on power and GND pins</t>
+  </si>
+  <si>
+    <t>No RF in design</t>
+  </si>
+  <si>
+    <t>Nedding evaluation for more test point placement and positioning</t>
+  </si>
+  <si>
+    <t>Added RoHS, still needs to verify PB Free, ESD not a concern in this design</t>
+  </si>
+  <si>
+    <t>Opted for manual soldering of the final board</t>
+  </si>
+  <si>
+    <t>Needing mechanical evalution</t>
+  </si>
+  <si>
+    <t>All 3D models available in a specific directory</t>
+  </si>
+  <si>
+    <t>Waiting further feedback on the current designators positioning and component placement</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1158,8 @@
   </sheetPr>
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1167,7 @@
     <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.140625" customWidth="1"/>
+    <col min="6" max="6" width="99" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -1110,7 +1182,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1133,7 +1205,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43965.840691550926</v>
+        <v>43974.854269444448</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1180,7 +1252,7 @@
         <v>133</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1196,7 +1268,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1212,7 +1284,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1228,7 +1300,7 @@
         <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1244,7 +1316,7 @@
         <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1260,7 +1332,7 @@
         <v>133</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,7 +1348,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,7 +1378,7 @@
         <v>133</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1322,7 +1394,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1338,7 +1410,7 @@
         <v>133</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1382,7 +1454,7 @@
         <v>133</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,7 +1484,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,7 +1514,7 @@
         <v>133</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1487,7 +1559,9 @@
         <v>133</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1496,10 +1570,10 @@
       <c r="B27" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
     </row>
@@ -1511,11 +1585,13 @@
         <v>95</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="7"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -1529,7 +1605,9 @@
         <v>133</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -1538,12 +1616,14 @@
       <c r="B30" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
@@ -1552,10 +1632,10 @@
       <c r="B31" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="7"/>
     </row>
@@ -1566,10 +1646,10 @@
       <c r="B32" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C32" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="7"/>
     </row>
@@ -1580,12 +1660,14 @@
       <c r="B33" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -1594,12 +1676,14 @@
       <c r="B34" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
@@ -1608,12 +1692,14 @@
       <c r="B35" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
@@ -1622,12 +1708,14 @@
       <c r="B36" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
@@ -1636,12 +1724,14 @@
       <c r="B37" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -1655,7 +1745,9 @@
       <c r="E38" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -1664,12 +1756,14 @@
       <c r="B39" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
@@ -1697,7 +1791,9 @@
       <c r="E41" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
@@ -1706,10 +1802,10 @@
       <c r="B42" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="7"/>
     </row>
@@ -1739,7 +1835,9 @@
         <v>133</v>
       </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -1753,7 +1851,9 @@
         <v>133</v>
       </c>
       <c r="E45" s="2"/>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1767,7 +1867,9 @@
       <c r="E46" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
@@ -1776,12 +1878,14 @@
       <c r="B47" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
@@ -1790,10 +1894,10 @@
       <c r="B48" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C48" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="7"/>
     </row>
@@ -1804,12 +1908,14 @@
       <c r="B49" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C49" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
@@ -1818,12 +1924,14 @@
       <c r="B50" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="7"/>
+      <c r="E50" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
@@ -1833,11 +1941,13 @@
         <v>118</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="7"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
@@ -1851,7 +1961,9 @@
         <v>133</v>
       </c>
       <c r="E52" s="2"/>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
@@ -1860,12 +1972,14 @@
       <c r="B53" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C53" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
@@ -1879,7 +1993,9 @@
         <v>133</v>
       </c>
       <c r="E54" s="2"/>
-      <c r="F54" s="7"/>
+      <c r="F54" s="7" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
@@ -1889,11 +2005,13 @@
         <v>123</v>
       </c>
       <c r="C55" s="2"/>
-      <c r="D55" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="7"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
@@ -1903,11 +2021,13 @@
         <v>121</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="7"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
@@ -1917,11 +2037,13 @@
         <v>128</v>
       </c>
       <c r="C57" s="2"/>
-      <c r="D57" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="7"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
@@ -1930,10 +2052,10 @@
       <c r="B58" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C58" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="F58" s="7"/>
     </row>
@@ -1949,7 +2071,9 @@
         <v>133</v>
       </c>
       <c r="E59" s="2"/>
-      <c r="F59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
@@ -1958,10 +2082,10 @@
       <c r="B60" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C60" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="F60" s="7"/>
     </row>

</xml_diff>

<commit_message>
Semi USB: checklist: Updating PCB Design Checklist for N.1 board, almost finished #18
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\1_Interface_Charge_RBF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA31E61C-648E-434C-BE43-4F16EB04F404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62602F65-C978-4B7A-8825-F456822443B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="197">
   <si>
     <t>1.</t>
   </si>
@@ -503,15 +503,9 @@
     <t>User's guide manual (PDF)</t>
   </si>
   <si>
-    <t>Variant: Semi USB - Charge and RBF Interstage Interface Board Nº1</t>
-  </si>
-  <si>
     <t>Since the PCB is a interface for flashing and debugging this is not needed</t>
   </si>
   <si>
-    <t>Done initial placement, waiting avaliation</t>
-  </si>
-  <si>
     <t>No Integrated Circuits in design</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>Power supply is provided by the msp-fet JTAG_VCC</t>
   </si>
   <si>
-    <t>Same used for the engeenering models</t>
-  </si>
-  <si>
     <t>Power from debugger must be stable enough</t>
   </si>
   <si>
@@ -548,27 +539,15 @@
     <t>Used direct contact on power and GND nets</t>
   </si>
   <si>
-    <t>See if the PCB manufacture have an acceptable hole size tolerance for connectors</t>
-  </si>
-  <si>
     <t>Just a bit off in the 3D models for the pin header but not critical</t>
   </si>
   <si>
     <t>Used polygons</t>
   </si>
   <si>
-    <t>Used standard 0.508mm to RBF and 0.254mm to all other ones (same as EPS module)</t>
-  </si>
-  <si>
     <t>Used at the moment 0.15mm from JLCPCB capabilities</t>
   </si>
   <si>
-    <t>Waiting final "martelada"</t>
-  </si>
-  <si>
-    <t>Simple 1,6mm thick double layer board design</t>
-  </si>
-  <si>
     <t>No analog and digital concerns for this simple board design</t>
   </si>
   <si>
@@ -578,9 +557,6 @@
     <t>Heavier components needs to be on top layer for AIT reasons</t>
   </si>
   <si>
-    <t>Needs some revision</t>
-  </si>
-  <si>
     <t>Project: Interstage Interface Panel for FloripaSat-2 CubeSat</t>
   </si>
   <si>
@@ -590,31 +566,64 @@
     <t>Extra empty column called "Board Layer Stack"</t>
   </si>
   <si>
-    <t>Only 1 plane GND on top layer used (2 layer design)</t>
-  </si>
-  <si>
     <t>Opted for direct contact on power and GND pins</t>
   </si>
   <si>
     <t>No RF in design</t>
   </si>
   <si>
-    <t>Nedding evaluation for more test point placement and positioning</t>
-  </si>
-  <si>
-    <t>Added RoHS, still needs to verify PB Free, ESD not a concern in this design</t>
-  </si>
-  <si>
-    <t>Opted for manual soldering of the final board</t>
-  </si>
-  <si>
     <t>Needing mechanical evalution</t>
   </si>
   <si>
     <t>All 3D models available in a specific directory</t>
   </si>
   <si>
-    <t>Waiting further feedback on the current designators positioning and component placement</t>
+    <t>Only two GND planes on both sides</t>
+  </si>
+  <si>
+    <t>Used polygons to Charge and power nets and 0.254mm to all other ones (same as EPS module)</t>
+  </si>
+  <si>
+    <t>Few components to be an advantage</t>
+  </si>
+  <si>
+    <t>Gabriel Mariano Marcelino</t>
+  </si>
+  <si>
+    <t>André Martins de Pio Mattos</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>Edemar Morsch Filho</t>
+  </si>
+  <si>
+    <t>Mechanical validadtion</t>
+  </si>
+  <si>
+    <t>Review and support</t>
+  </si>
+  <si>
+    <t>Done initial placement "aproved"</t>
+  </si>
+  <si>
+    <t>Variant: Semi USB - "Charge" Board Nº1</t>
+  </si>
+  <si>
+    <t>Same used for the enginnering models</t>
+  </si>
+  <si>
+    <t>"Aproved"</t>
+  </si>
+  <si>
+    <t>Simple 1,6mm thick double layer board design, details in altium are not relevant to manufacture</t>
+  </si>
+  <si>
+    <t>Space PCBs are not RoHS compilant</t>
+  </si>
+  <si>
+    <t>Initialy to be done in JLCPCB</t>
   </si>
 </sst>
 </file>
@@ -1156,10 +1165,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1191,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -1196,7 +1205,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1205,7 +1214,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>43974.854269444448</v>
+        <v>44013.442795949071</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1252,7 +1261,7 @@
         <v>133</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1262,13 +1271,13 @@
       <c r="B7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1278,13 +1287,13 @@
       <c r="B8" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F8" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,7 +1309,7 @@
         <v>133</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1316,7 +1325,7 @@
         <v>133</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1332,7 +1341,7 @@
         <v>133</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1348,7 +1357,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1378,7 +1387,7 @@
         <v>133</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1394,7 +1403,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="7" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,7 +1419,7 @@
         <v>133</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,7 +1463,7 @@
         <v>133</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1478,13 +1487,13 @@
       <c r="B21" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F21" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1514,7 +1523,7 @@
         <v>133</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,7 +1569,7 @@
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,7 +1599,7 @@
         <v>133</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1600,14 +1609,12 @@
       <c r="B29" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="7" t="s">
-        <v>171</v>
-      </c>
+      <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
@@ -1622,7 +1629,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="7" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1666,7 +1673,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="7" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1682,7 +1689,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="7" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1698,7 +1705,7 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="7" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1714,7 +1721,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="7" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1730,7 +1737,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="7" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1746,7 +1753,7 @@
         <v>133</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1762,7 +1769,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="7" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1792,7 +1799,7 @@
         <v>133</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1830,14 +1837,12 @@
       <c r="B44" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C44" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="7" t="s">
-        <v>181</v>
-      </c>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -1846,14 +1851,12 @@
       <c r="B45" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C45" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="7" t="s">
-        <v>193</v>
-      </c>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1868,7 +1871,7 @@
         <v>133</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1884,7 +1887,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1894,10 +1897,10 @@
       <c r="B48" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="E48" s="2"/>
       <c r="F48" s="7"/>
     </row>
@@ -1908,13 +1911,13 @@
       <c r="B49" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F49" s="7" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1924,14 +1927,12 @@
       <c r="B50" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>190</v>
-      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
@@ -1940,14 +1941,12 @@
       <c r="B51" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>190</v>
-      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
@@ -1956,14 +1955,12 @@
       <c r="B52" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C52" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="7" t="s">
-        <v>191</v>
-      </c>
+      <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
@@ -1978,7 +1975,7 @@
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="F53" s="7" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1988,13 +1985,13 @@
       <c r="B54" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C54" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="7" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2010,7 +2007,7 @@
         <v>133</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2026,7 +2023,7 @@
         <v>133</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2042,7 +2039,7 @@
         <v>133</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,14 +2063,12 @@
       <c r="B59" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C59" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="7" t="s">
-        <v>188</v>
-      </c>
+      <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
@@ -2097,11 +2092,13 @@
         <v>127</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="7"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
@@ -2110,12 +2107,14 @@
       <c r="B62" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
-        <v>133</v>
-      </c>
+      <c r="C62" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="7"/>
+      <c r="F62" s="7" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
@@ -2267,10 +2266,10 @@
         <v>144</v>
       </c>
       <c r="C73" s="2"/>
-      <c r="D73" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E73" s="2"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2331,8 +2330,12 @@
       <c r="A78" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="17"/>
+      <c r="B78" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>189</v>
+      </c>
       <c r="D78" s="18"/>
       <c r="E78" s="19"/>
       <c r="F78" s="14"/>
@@ -2341,14 +2344,33 @@
       <c r="A79" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="17"/>
+      <c r="B79" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>189</v>
+      </c>
       <c r="D79" s="18"/>
       <c r="E79" s="19"/>
       <c r="F79" s="14"/>
     </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D80" s="18"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="C80:E80"/>
     <mergeCell ref="C77:E77"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C79:E79"/>

</xml_diff>

<commit_message>
Semi USB: checklist: Finished PCB Design Checklist for N.1 board close #18
</commit_message>
<xml_diff>
--- a/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
+++ b/semi_usb_interface/Source of all boards/1_Interface_Charge_RBF/PCB Design Checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanaz\OneDrive\Área de Trabalho\SpaceLab\FloripaSat-2\Hardware Development\interface-board\semi_usb_interface\Source of all boards\1_Interface_Charge_RBF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62602F65-C978-4B7A-8825-F456822443B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B34614-628E-4AE1-A08B-1CFAEE98E70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5735AEBB-7E66-4CF4-B607-EA3656031333}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="198">
   <si>
     <t>1.</t>
   </si>
@@ -599,18 +599,12 @@
     <t>Edemar Morsch Filho</t>
   </si>
   <si>
-    <t>Mechanical validadtion</t>
-  </si>
-  <si>
     <t>Review and support</t>
   </si>
   <si>
     <t>Done initial placement "aproved"</t>
   </si>
   <si>
-    <t>Variant: Semi USB - "Charge" Board Nº1</t>
-  </si>
-  <si>
     <t>Same used for the enginnering models</t>
   </si>
   <si>
@@ -624,6 +618,15 @@
   </si>
   <si>
     <t>Initialy to be done in JLCPCB</t>
+  </si>
+  <si>
+    <t>Variant: Semi USB - "IIP_Charge" Board Nº1</t>
+  </si>
+  <si>
+    <t>Under development</t>
+  </si>
+  <si>
+    <t>Mechanical validation</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1170,8 @@
   </sheetPr>
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1208,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1214,7 +1217,7 @@
       </c>
       <c r="E3" s="9">
         <f ca="1">NOW()</f>
-        <v>44013.442795949071</v>
+        <v>44023.946729282405</v>
       </c>
       <c r="F3" s="7"/>
     </row>
@@ -1277,7 +1280,7 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,7 +1406,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1721,7 +1724,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1740,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1917,7 +1920,7 @@
         <v>133</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2113,7 +2116,7 @@
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2153,10 +2156,10 @@
       <c r="B65" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C65" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" s="1"/>
       <c r="E65" s="2"/>
       <c r="F65" s="3"/>
     </row>
@@ -2167,10 +2170,10 @@
       <c r="B66" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="1"/>
       <c r="E66" s="2"/>
       <c r="F66" s="3"/>
     </row>
@@ -2182,10 +2185,10 @@
         <v>139</v>
       </c>
       <c r="C67" s="2"/>
-      <c r="D67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E67" s="2"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F67" s="3"/>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2195,10 +2198,10 @@
       <c r="B68" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C68" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" s="1"/>
       <c r="E68" s="2"/>
       <c r="F68" s="3"/>
     </row>
@@ -2209,10 +2212,10 @@
       <c r="B69" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C69" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D69" s="1"/>
       <c r="E69" s="2"/>
       <c r="F69" s="3"/>
     </row>
@@ -2223,10 +2226,10 @@
       <c r="B70" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="2"/>
-      <c r="D70" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C70" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D70" s="1"/>
       <c r="E70" s="2"/>
       <c r="F70" s="3"/>
     </row>
@@ -2237,10 +2240,10 @@
       <c r="B71" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C71" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="1"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
     </row>
@@ -2251,10 +2254,10 @@
       <c r="B72" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="C72" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D72" s="1"/>
       <c r="E72" s="2"/>
       <c r="F72" s="3"/>
     </row>
@@ -2284,7 +2287,9 @@
         <v>133</v>
       </c>
       <c r="E74" s="2"/>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
@@ -2334,7 +2339,7 @@
         <v>184</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="19"/>
@@ -2348,7 +2353,7 @@
         <v>185</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D79" s="18"/>
       <c r="E79" s="19"/>
@@ -2362,7 +2367,7 @@
         <v>187</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="19"/>

</xml_diff>